<commit_message>
feat: Add customer loan count metrics + CAC per loan amortization
</commit_message>
<xml_diff>
--- a/data/exports/fct_cohort_performance.xlsx
+++ b/data/exports/fct_cohort_performance.xlsx
@@ -631,7 +631,7 @@
         <v>52695.52</v>
       </c>
       <c r="K2" t="n">
-        <v>177.4196705559368</v>
+        <v>177.4196705559369</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -649,7 +649,7 @@
         <v>258120.0084129709</v>
       </c>
       <c r="Q2" t="n">
-        <v>177.4196705559368</v>
+        <v>177.4196705559369</v>
       </c>
       <c r="R2" t="n">
         <v>177.1585507295614</v>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9985282363248829</v>
+        <v>0.9985282363248826</v>
       </c>
       <c r="U2" t="n">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>716</v>
+        <v>1140</v>
       </c>
       <c r="Y2" t="n">
         <v>0</v>
@@ -682,7 +682,7 @@
         <v>1032260.03</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.491420716047287</v>
+        <v>0.7824296355247498</v>
       </c>
       <c r="AC2" t="n">
         <v>0.119423471391201</v>
@@ -691,7 +691,7 @@
         <v>258120.0084129709</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.256963132074388</v>
+        <v>1.203780779789366</v>
       </c>
       <c r="AF2" t="n">
         <v>7.437406824612079</v>
@@ -727,7 +727,7 @@
         <v>8808.08</v>
       </c>
       <c r="I3" t="n">
-        <v>7740.43</v>
+        <v>7740.429999999998</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>7217.822999999999</v>
+        <v>7217.823</v>
       </c>
       <c r="O3" t="n">
         <v>8808.08</v>
@@ -772,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>129948.32</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.9223300814628601</v>
+        <v>1</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -793,10 +793,10 @@
         <v>8808.08</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.5430192140824555</v>
+        <v>0.5430192140824556</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.220323634979689</v>
+        <v>1.220323634979688</v>
       </c>
     </row>
     <row r="4">
@@ -817,7 +817,7 @@
         <v>430</v>
       </c>
       <c r="E4" t="n">
-        <v>836425.4000000001</v>
+        <v>836425.4</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -829,7 +829,7 @@
         <v>107121.92</v>
       </c>
       <c r="I4" t="n">
-        <v>84780.07000000001</v>
+        <v>84780.06999999999</v>
       </c>
       <c r="J4" t="n">
         <v>9357.459999999999</v>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9997304604276773</v>
+        <v>0.9997304604276772</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>408</v>
+        <v>547</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
@@ -883,10 +883,10 @@
         <v>11</v>
       </c>
       <c r="AA4" t="n">
-        <v>716567.23</v>
+        <v>716567.2300000001</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.7145358920097351</v>
+        <v>0.9579684734344482</v>
       </c>
       <c r="AC4" t="n">
         <v>0.01926444843411446</v>
@@ -895,10 +895,10 @@
         <v>107093.0464034968</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.6396713225928637</v>
+        <v>0.6544808264905551</v>
       </c>
       <c r="AF4" t="n">
-        <v>4.213231128770637</v>
+        <v>4.213231128770636</v>
       </c>
     </row>
     <row r="5">
@@ -1074,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y6" t="n">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>11722.87</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.625</v>
+        <v>1</v>
       </c>
       <c r="AC6" t="n">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         <v>1579</v>
       </c>
       <c r="E7" t="n">
-        <v>2545370.779999999</v>
+        <v>2545370.78</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1128,10 +1128,10 @@
         <v>1074.903201013513</v>
       </c>
       <c r="H7" t="n">
-        <v>496462.9100000001</v>
+        <v>496462.91</v>
       </c>
       <c r="I7" t="n">
-        <v>340922.62</v>
+        <v>340922.6199999999</v>
       </c>
       <c r="J7" t="n">
         <v>95363.36</v>
@@ -1149,22 +1149,22 @@
         <v>52107.251</v>
       </c>
       <c r="O7" t="n">
-        <v>496462.9100000001</v>
+        <v>496462.91</v>
       </c>
       <c r="P7" t="n">
-        <v>495954.6266797294</v>
+        <v>495954.6266797292</v>
       </c>
       <c r="Q7" t="n">
         <v>209.6549451013514</v>
       </c>
       <c r="R7" t="n">
-        <v>209.4402984289398</v>
+        <v>209.4402984289397</v>
       </c>
       <c r="S7" t="n">
         <v>1</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9989761907485278</v>
+        <v>0.9989761907485277</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
@@ -1176,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="X7" t="n">
-        <v>835</v>
+        <v>2003</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
@@ -1188,19 +1188,19 @@
         <v>1795890.34</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.3526182472705841</v>
+        <v>0.8458614945411682</v>
       </c>
       <c r="AC7" t="n">
         <v>0.02913851290941238</v>
       </c>
       <c r="AD7" t="n">
-        <v>495954.6266797294</v>
+        <v>495954.6266797292</v>
       </c>
       <c r="AE7" t="n">
-        <v>1.429697740639335</v>
+        <v>1.454724483175093</v>
       </c>
       <c r="AF7" t="n">
-        <v>9.517958003190946</v>
+        <v>9.517958003190941</v>
       </c>
     </row>
     <row r="8">
@@ -1239,7 +1239,7 @@
         <v>58</v>
       </c>
       <c r="K8" t="n">
-        <v>78.0022767857143</v>
+        <v>78.00227678571427</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -1257,10 +1257,10 @@
         <v>17472.51</v>
       </c>
       <c r="Q8" t="n">
-        <v>78.0022767857143</v>
+        <v>78.00227678571427</v>
       </c>
       <c r="R8" t="n">
-        <v>78.0022767857143</v>
+        <v>78.00227678571427</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>165</v>
+        <v>224</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -1290,7 +1290,7 @@
         <v>248950.2</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.7366071343421936</v>
+        <v>1</v>
       </c>
       <c r="AC8" t="n">
         <v>0</v>
@@ -1302,7 +1302,7 @@
         <v>0.341349267676323</v>
       </c>
       <c r="AF8" t="n">
-        <v>1.93957445056014</v>
+        <v>1.939574450560139</v>
       </c>
     </row>
     <row r="9">
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1412.026268518519</v>
+        <v>1412.026268518518</v>
       </c>
       <c r="H9" t="n">
-        <v>231028.5099999999</v>
+        <v>231028.51</v>
       </c>
       <c r="I9" t="n">
         <v>184806.01</v>
@@ -1350,10 +1350,10 @@
         <v>30.43612696233116</v>
       </c>
       <c r="N9" t="n">
-        <v>41511.6055</v>
+        <v>41511.60550000001</v>
       </c>
       <c r="O9" t="n">
-        <v>231028.5099999999</v>
+        <v>231028.51</v>
       </c>
       <c r="P9" t="n">
         <v>230998.0738730376</v>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9998682581341918</v>
+        <v>0.9998682581341914</v>
       </c>
       <c r="U9" t="n">
         <v>0</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>556</v>
+        <v>1062</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>1380204.43</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.5148147940635681</v>
+        <v>0.9833333492279053</v>
       </c>
       <c r="AC9" t="n">
         <v>0.0009259259095415473</v>
@@ -1401,7 +1401,7 @@
         <v>230998.0738730376</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.858112888272384</v>
+        <v>0.8382440498110526</v>
       </c>
       <c r="AF9" t="n">
         <v>5.564662486326568</v>
@@ -1434,7 +1434,7 @@
         <v>1082.235</v>
       </c>
       <c r="H10" t="n">
-        <v>813.3200000000001</v>
+        <v>813.3199999999999</v>
       </c>
       <c r="I10" t="n">
         <v>714.73</v>
@@ -1455,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>813.3200000000001</v>
+        <v>813.3199999999999</v>
       </c>
       <c r="P10" t="n">
-        <v>813.3200000000001</v>
+        <v>813.3199999999999</v>
       </c>
       <c r="Q10" t="n">
         <v>203.33</v>
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y10" t="n">
         <v>0</v>
@@ -1494,13 +1494,13 @@
         <v>4328.94</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>813.3200000000001</v>
+        <v>813.3199999999999</v>
       </c>
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" t="inlineStr"/>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="Y11" t="n">
         <v>0</v>
@@ -1592,7 +1592,7 @@
         <v>31029.37</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.7222222089767456</v>
+        <v>1</v>
       </c>
       <c r="AC11" t="n">
         <v>0</v>
@@ -1682,7 +1682,7 @@
         <v>0.001385041512548923</v>
       </c>
       <c r="X12" t="n">
-        <v>251</v>
+        <v>1936</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -1694,7 +1694,7 @@
         <v>1609925.75</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.1158818081021309</v>
+        <v>0.8938134908676147</v>
       </c>
       <c r="AC12" t="n">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>426450.1746825942</v>
       </c>
       <c r="AE12" t="n">
-        <v>1.350367217979932</v>
+        <v>1.343816377676004</v>
       </c>
       <c r="AF12" t="n">
         <v>15.51587628536336</v>
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>4709.800499999999</v>
+        <v>4709.8005</v>
       </c>
       <c r="O13" t="n">
         <v>25373.01</v>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>52</v>
+        <v>240</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
         <v>335728.04</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.2166666686534882</v>
+        <v>1</v>
       </c>
       <c r="AC13" t="n">
         <v>0</v>
@@ -1808,7 +1808,7 @@
         <v>0.1746228070175438</v>
       </c>
       <c r="AF13" t="n">
-        <v>5.387279142715282</v>
+        <v>5.387279142715281</v>
       </c>
     </row>
     <row r="14">
@@ -1841,7 +1841,7 @@
         <v>208429.96</v>
       </c>
       <c r="I14" t="n">
-        <v>168572.5399999999</v>
+        <v>168572.54</v>
       </c>
       <c r="J14" t="n">
         <v>14593.14</v>
@@ -1874,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9998539743184602</v>
+        <v>0.99985397431846</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>157</v>
+        <v>1111</v>
       </c>
       <c r="Y14" t="n">
         <v>0</v>
@@ -1898,7 +1898,7 @@
         <v>1281887.13</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.1384479701519012</v>
+        <v>0.9797177910804749</v>
       </c>
       <c r="AC14" t="n">
         <v>0</v>
@@ -1907,7 +1907,7 @@
         <v>208399.5238730377</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.5533988446269038</v>
+        <v>0.553283102621172</v>
       </c>
       <c r="AF14" t="n">
         <v>7.867956357774902</v>
@@ -1937,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>906.2245454545456</v>
+        <v>906.2245454545454</v>
       </c>
       <c r="H15" t="n">
         <v>3079.94</v>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="X15" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="Y15" t="n">
         <v>0</v>
@@ -2000,7 +2000,7 @@
         <v>19249.23</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.09090909361839294</v>
+        <v>1</v>
       </c>
       <c r="AC15" t="n">
         <v>0</v>

</xml_diff>